<commit_message>
done mflop calc for part a
Signed-off-by: Aaron <10177767+AaronPinto@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Assignment 2/timing/a2.xlsx
+++ b/Assignment 2/timing/a2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\raeedh\school\COMPENG4DM4\Assignment 2\timing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\4th Year\4DM4\Assignment 2\timing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD7ED91D-4461-4F75-A009-FDCEDB740441}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24A2FF04-4D8B-41A1-95F4-12FD905D284D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-21720" windowWidth="51840" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2a" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1473" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1474" uniqueCount="244">
   <si>
     <t>4DM4 Assignment 2(a), DAXPY Loop, No Unrolling, No Scheduling</t>
     <phoneticPr fontId="0" type="noConversion"/>
@@ -813,13 +813,29 @@
   </si>
   <si>
     <t>4DM4 Assignment 2(e), DAXPY Loop, Unrolling, Scheduling, On Dual-Issue Machine</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">20cc per iteration of the loop, 2 FLOPs per iteration (MULT.D &amp; ADD.D), therefore 2 FLOP/20cc. (3 GHz)*(2 FLOP/20cc) = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>300 MFLOP/sec</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="26" x14ac:knownFonts="1">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -982,6 +998,14 @@
       <color theme="5"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1286,7 +1310,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1414,6 +1438,9 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1703,8 +1730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:AA40"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2541,6 +2568,20 @@
       <c r="B29" t="s">
         <v>31</v>
       </c>
+      <c r="C29" s="94" t="s">
+        <v>243</v>
+      </c>
+      <c r="D29" s="94"/>
+      <c r="E29" s="94"/>
+      <c r="F29" s="94"/>
+      <c r="G29" s="94"/>
+      <c r="H29" s="94"/>
+      <c r="I29" s="94"/>
+      <c r="J29" s="94"/>
+      <c r="K29" s="94"/>
+      <c r="L29" s="94"/>
+      <c r="M29" s="94"/>
+      <c r="N29" s="94"/>
     </row>
     <row r="30" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
@@ -2567,7 +2608,11 @@
       <c r="R40" s="17"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C29:N29"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2575,8 +2620,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02356681-9A30-45C3-BE25-535E5C1A58D7}">
   <dimension ref="B2:AA40"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:B10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19861,7 +19906,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5B3E4D6-082C-4FC5-9A0B-7416C52470AD}">
   <dimension ref="A2:N32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
done mflop calc for all parts + part b comments
Signed-off-by: Aaron <10177767+AaronPinto@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Assignment 2/timing/a2.xlsx
+++ b/Assignment 2/timing/a2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\4th Year\4DM4\Assignment 2\timing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24A2FF04-4D8B-41A1-95F4-12FD905D284D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0741031C-04FD-4219-920A-D2D215029BF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-21720" windowWidth="51840" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-21720" windowWidth="51840" windowHeight="21240" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2a" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1474" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1485" uniqueCount="249">
   <si>
     <t>4DM4 Assignment 2(a), DAXPY Loop, No Unrolling, No Scheduling</t>
     <phoneticPr fontId="0" type="noConversion"/>
@@ -830,12 +830,79 @@
       <t>300 MFLOP/sec</t>
     </r>
   </si>
+  <si>
+    <t>forward R1 (EX* to *EX) in cc8</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">18cc per iteration of the loop, 2 FLOPs per iteration (MULT.D &amp; ADD.D), therefore 2 FLOP/18cc. (3 GHz)*(2 FLOP/18cc) = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>333.3 MFLOP/sec</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">62cc per unrolled iteration of the loop, 8 FLOPs per iteration (MULT.D &amp; ADD.D), therefore 8 FLOP/62cc. (3 GHz)*(8 FLOP/62cc) = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>387.1 MFLOP/sec</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">29cc per iteration of the loop, 8 FLOPs per iteration (MULT.D &amp; ADD.D), therefore 8 FLOP/29cc. (3 GHz)*(8 FLOP/29cc) = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>827.6 MFLOP/sec</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">22cc per iteration of the loop, 8 FLOPs per iteration (MULT.D &amp; ADD.D), therefore 8 FLOP/22cc. (3 GHz)*(8 FLOP/22cc) = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1090.9 MFLOP/sec</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="27" x14ac:knownFonts="1">
+  <fonts count="29" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1003,6 +1070,21 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1310,7 +1392,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1442,6 +1524,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1731,7 +1817,7 @@
   <dimension ref="B2:AA40"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+      <selection activeCell="C29" sqref="C29:N29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1996,7 +2082,7 @@
       <c r="X14" s="11"/>
       <c r="Y14" s="11"/>
       <c r="Z14" s="11"/>
-      <c r="AA14" s="12" t="s">
+      <c r="AA14" s="9" t="s">
         <v>41</v>
       </c>
     </row>
@@ -2620,8 +2706,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02356681-9A30-45C3-BE25-535E5C1A58D7}">
   <dimension ref="B2:AA40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29:N29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2888,7 +2974,9 @@
       <c r="X14" s="11"/>
       <c r="Y14" s="11"/>
       <c r="Z14" s="11"/>
-      <c r="AA14" s="12"/>
+      <c r="AA14" s="9" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="15" spans="2:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B15" s="9" t="s">
@@ -2984,7 +3072,9 @@
       <c r="X16" s="11"/>
       <c r="Y16" s="11"/>
       <c r="Z16" s="11"/>
-      <c r="AA16" s="9"/>
+      <c r="AA16" s="9" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="17" spans="2:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B17" s="9" t="s">
@@ -3026,7 +3116,9 @@
       <c r="X17" s="11"/>
       <c r="Y17" s="11"/>
       <c r="Z17" s="11"/>
-      <c r="AA17" s="9"/>
+      <c r="AA17" s="9" t="s">
+        <v>244</v>
+      </c>
     </row>
     <row r="18" spans="2:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B18" s="9" t="s">
@@ -3405,12 +3497,24 @@
       <c r="U28" s="16"/>
       <c r="V28" s="16"/>
     </row>
-    <row r="29" spans="2:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>31</v>
       </c>
-      <c r="D29" s="25"/>
-      <c r="E29" s="26"/>
+      <c r="C29" s="94" t="s">
+        <v>245</v>
+      </c>
+      <c r="D29" s="94"/>
+      <c r="E29" s="94"/>
+      <c r="F29" s="94"/>
+      <c r="G29" s="94"/>
+      <c r="H29" s="94"/>
+      <c r="I29" s="94"/>
+      <c r="J29" s="94"/>
+      <c r="K29" s="94"/>
+      <c r="L29" s="94"/>
+      <c r="M29" s="94"/>
+      <c r="N29" s="94"/>
     </row>
     <row r="30" spans="2:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
@@ -3467,6 +3571,9 @@
       <c r="R40" s="17"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C29:N29"/>
+  </mergeCells>
   <conditionalFormatting sqref="C19:Z26 C18:E18 G18:Z18 C14:Z17">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"stall"</formula>
@@ -3480,8 +3587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2947B3F-865E-4E46-9A91-E9BDDBBE8BD5}">
   <dimension ref="B2:DC49"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:B10"/>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48:O48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8155,6 +8262,21 @@
       <c r="B48" t="s">
         <v>31</v>
       </c>
+      <c r="C48" s="96" t="s">
+        <v>246</v>
+      </c>
+      <c r="D48" s="96"/>
+      <c r="E48" s="96"/>
+      <c r="F48" s="96"/>
+      <c r="G48" s="96"/>
+      <c r="H48" s="96"/>
+      <c r="I48" s="96"/>
+      <c r="J48" s="96"/>
+      <c r="K48" s="96"/>
+      <c r="L48" s="96"/>
+      <c r="M48" s="96"/>
+      <c r="N48" s="96"/>
+      <c r="O48" s="96"/>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
@@ -8162,16 +8284,19 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C48:O48"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{787CC242-34F4-4FF7-A40F-1653B5D3686C}">
-  <dimension ref="A1:J42"/>
+  <dimension ref="A1:O42"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40:O40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9258,7 +9383,7 @@
       </c>
       <c r="H32" s="34"/>
     </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B33" s="33" t="s">
         <v>28</v>
       </c>
@@ -9280,7 +9405,7 @@
       </c>
       <c r="H33" s="34"/>
     </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B34" s="33" t="s">
         <v>29</v>
       </c>
@@ -9301,7 +9426,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B35" s="33" t="s">
         <v>30</v>
       </c>
@@ -9320,7 +9445,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B36" s="33" t="s">
         <v>45</v>
       </c>
@@ -9335,7 +9460,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B37" s="34" t="s">
         <v>45</v>
       </c>
@@ -9350,22 +9475,37 @@
         <v>108</v>
       </c>
     </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C38" s="43"/>
       <c r="D38" s="43"/>
       <c r="E38" s="43"/>
       <c r="F38" s="43"/>
       <c r="G38" s="43"/>
     </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C40" s="96" t="s">
+        <v>246</v>
+      </c>
+      <c r="D40" s="96"/>
+      <c r="E40" s="96"/>
+      <c r="F40" s="96"/>
+      <c r="G40" s="96"/>
+      <c r="H40" s="96"/>
+      <c r="I40" s="96"/>
+      <c r="J40" s="96"/>
+      <c r="K40" s="96"/>
+      <c r="L40" s="96"/>
+      <c r="M40" s="96"/>
+      <c r="N40" s="96"/>
+      <c r="O40" s="96"/>
+    </row>
+    <row r="41" spans="2:15" x14ac:dyDescent="0.25">
       <c r="H41" s="37"/>
     </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>61</v>
       </c>
@@ -9374,6 +9514,9 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C40:O40"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -9382,8 +9525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA4769AE-CF13-4E3F-A6FE-AC5700114344}">
   <dimension ref="B2:DC77"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48:N48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13774,190 +13917,207 @@
       <c r="B48" t="s">
         <v>31</v>
       </c>
-      <c r="G48" s="9" t="s">
+      <c r="C48" s="94" t="s">
+        <v>247</v>
+      </c>
+      <c r="D48" s="94"/>
+      <c r="E48" s="94"/>
+      <c r="F48" s="94"/>
+      <c r="G48" s="94"/>
+      <c r="H48" s="94"/>
+      <c r="I48" s="94"/>
+      <c r="J48" s="94"/>
+      <c r="K48" s="94"/>
+      <c r="L48" s="94"/>
+      <c r="M48" s="94"/>
+      <c r="N48" s="94"/>
+      <c r="R48" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="K48" s="9" t="s">
+      <c r="V48" s="9" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="49" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>32</v>
       </c>
-      <c r="G49" s="9" t="s">
+      <c r="R49" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="K49" s="9" t="s">
+      <c r="V49" s="9" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="50" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="G50" s="9" t="s">
+    <row r="50" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="R50" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="K50" s="9" t="s">
+      <c r="V50" s="9" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="51" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="G51" s="9" t="s">
+    <row r="51" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="R51" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="K51" s="9" t="s">
+      <c r="V51" s="9" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="52" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="G52" s="9" t="s">
+    <row r="52" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="R52" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="K52" s="9" t="s">
+      <c r="V52" s="9" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="53" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="G53" s="9" t="s">
+    <row r="53" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="R53" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="K53" s="9" t="s">
+      <c r="V53" s="9" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="54" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="G54" s="9" t="s">
+    <row r="54" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="R54" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="K54" s="9" t="s">
+      <c r="V54" s="9" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="55" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="G55" s="9" t="s">
+    <row r="55" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="R55" s="9" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="56" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="G56" s="9" t="s">
+    <row r="56" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="R56" s="9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="57" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="G57" s="9" t="s">
+    <row r="57" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="R57" s="9" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="58" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="G58" s="9" t="s">
+    <row r="58" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="R58" s="9" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="59" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="G59" s="9" t="s">
+    <row r="59" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="R59" s="9" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="60" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="G60" s="9" t="s">
+    <row r="60" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="R60" s="9" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="61" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="G61" s="9" t="s">
+    <row r="61" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="R61" s="9" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="62" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="G62" s="9" t="s">
+    <row r="62" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="R62" s="9" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="63" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="G63" s="9" t="s">
+    <row r="63" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="R63" s="9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="64" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="G64" s="9" t="s">
+    <row r="64" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="R64" s="9" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="65" spans="7:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="G65" s="9" t="s">
+    <row r="65" spans="18:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="R65" s="9" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="66" spans="7:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="G66" s="9" t="s">
+    <row r="66" spans="18:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="R66" s="9" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="67" spans="7:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="G67" s="9" t="s">
+    <row r="67" spans="18:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="R67" s="9" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="68" spans="7:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="G68" s="9" t="s">
+    <row r="68" spans="18:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="R68" s="9" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="69" spans="7:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="G69" s="9" t="s">
+    <row r="69" spans="18:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="R69" s="9" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="70" spans="7:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="G70" s="9" t="s">
+    <row r="70" spans="18:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="R70" s="9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="71" spans="7:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="G71" s="9" t="s">
+    <row r="71" spans="18:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="R71" s="9" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="72" spans="7:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="G72" s="9" t="s">
+    <row r="72" spans="18:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="R72" s="9" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="73" spans="7:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="G73" s="9" t="s">
+    <row r="73" spans="18:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="R73" s="9" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="74" spans="7:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="G74" s="9" t="s">
+    <row r="74" spans="18:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="R74" s="9" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="75" spans="7:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="G75" s="9" t="s">
+    <row r="75" spans="18:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="R75" s="9" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="76" spans="7:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="G76" s="9" t="s">
+    <row r="76" spans="18:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="R76" s="9" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="77" spans="7:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="G77" s="9" t="s">
+    <row r="77" spans="18:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="R77" s="9" t="s">
         <v>30</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C48:N48"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E84740D-9A84-4CFB-977F-D74F74FE9540}">
-  <dimension ref="A1:J34"/>
+  <dimension ref="A1:N34"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14676,7 +14836,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B17" s="33" t="s">
         <v>133</v>
       </c>
@@ -14698,7 +14858,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B18" s="33" t="s">
         <v>130</v>
       </c>
@@ -14720,7 +14880,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B19" s="33" t="s">
         <v>29</v>
       </c>
@@ -14740,7 +14900,7 @@
       </c>
       <c r="H19" s="34"/>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B20" s="33" t="s">
         <v>124</v>
       </c>
@@ -14760,7 +14920,7 @@
       </c>
       <c r="H20" s="34"/>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B21" s="33" t="s">
         <v>134</v>
       </c>
@@ -14781,7 +14941,7 @@
       </c>
       <c r="H21" s="44"/>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B22" s="33" t="s">
         <v>135</v>
       </c>
@@ -14802,7 +14962,7 @@
       </c>
       <c r="H22" s="34"/>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B23" s="33" t="s">
         <v>136</v>
       </c>
@@ -14823,7 +14983,7 @@
       </c>
       <c r="H23" s="44"/>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B24" s="33" t="s">
         <v>125</v>
       </c>
@@ -14846,7 +15006,7 @@
       </c>
       <c r="H24" s="34"/>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B25" s="33" t="s">
         <v>137</v>
       </c>
@@ -14869,7 +15029,7 @@
       </c>
       <c r="H25" s="34"/>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B26" s="33" t="s">
         <v>138</v>
       </c>
@@ -14892,7 +15052,7 @@
       </c>
       <c r="H26" s="34"/>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B27" s="33" t="s">
         <v>30</v>
       </c>
@@ -14908,7 +15068,7 @@
       <c r="G27" s="35"/>
       <c r="H27" s="34"/>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B28" s="33" t="s">
         <v>139</v>
       </c>
@@ -14930,7 +15090,7 @@
       </c>
       <c r="H28" s="44"/>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B29" s="33" t="s">
         <v>140</v>
       </c>
@@ -14950,17 +15110,31 @@
       </c>
       <c r="H29" s="34"/>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C30" s="43"/>
       <c r="D30" s="43"/>
       <c r="E30" s="43"/>
       <c r="F30" s="43"/>
       <c r="G30" s="43"/>
     </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>60</v>
       </c>
+      <c r="C32" s="94" t="s">
+        <v>247</v>
+      </c>
+      <c r="D32" s="94"/>
+      <c r="E32" s="94"/>
+      <c r="F32" s="94"/>
+      <c r="G32" s="94"/>
+      <c r="H32" s="94"/>
+      <c r="I32" s="94"/>
+      <c r="J32" s="94"/>
+      <c r="K32" s="94"/>
+      <c r="L32" s="94"/>
+      <c r="M32" s="94"/>
+      <c r="N32" s="94"/>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="H33" s="37"/>
@@ -14974,6 +15148,9 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C32:N32"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -14982,8 +15159,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{238898DC-EDD0-4084-9AC1-82019E5FBD6F}">
   <dimension ref="B2:DC77"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48:N48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19520,281 +19697,278 @@
       <c r="B48" t="s">
         <v>31</v>
       </c>
-      <c r="F48" s="63"/>
-      <c r="G48" s="9" t="s">
+      <c r="C48" s="95" t="s">
+        <v>248</v>
+      </c>
+      <c r="D48" s="95"/>
+      <c r="E48" s="95"/>
+      <c r="F48" s="95"/>
+      <c r="G48" s="95"/>
+      <c r="H48" s="95"/>
+      <c r="I48" s="95"/>
+      <c r="J48" s="95"/>
+      <c r="K48" s="95"/>
+      <c r="L48" s="95"/>
+      <c r="M48" s="95"/>
+      <c r="N48" s="95"/>
+      <c r="U48" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="H48" s="5"/>
-      <c r="I48" s="5"/>
-      <c r="J48" s="9" t="s">
+      <c r="V48" s="5"/>
+      <c r="W48" s="5"/>
+      <c r="X48" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="K48" s="9" t="s">
+      <c r="Y48" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="L48" s="63"/>
-      <c r="M48" s="63"/>
-      <c r="N48" s="63"/>
-    </row>
-    <row r="49" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Z48" s="63"/>
+      <c r="AA48" s="63"/>
+    </row>
+    <row r="49" spans="2:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>32</v>
       </c>
       <c r="F49" s="63"/>
-      <c r="G49" s="9" t="s">
+      <c r="U49" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="H49" s="5"/>
-      <c r="I49" s="5"/>
-      <c r="J49" s="9" t="s">
+      <c r="V49" s="5"/>
+      <c r="W49" s="5"/>
+      <c r="X49" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="K49" s="9" t="s">
+      <c r="Y49" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="L49" s="63"/>
-      <c r="M49" s="63"/>
-      <c r="N49" s="63"/>
-    </row>
-    <row r="50" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Z49" s="63"/>
+      <c r="AA49" s="63"/>
+    </row>
+    <row r="50" spans="2:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="F50" s="63"/>
-      <c r="G50" s="9" t="s">
+      <c r="U50" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="H50" s="5"/>
-      <c r="I50" s="5"/>
-      <c r="J50" s="9" t="s">
+      <c r="V50" s="5"/>
+      <c r="W50" s="5"/>
+      <c r="X50" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="K50" s="9" t="s">
+      <c r="Y50" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="L50" s="63"/>
-      <c r="M50" s="63"/>
-      <c r="N50" s="63"/>
-    </row>
-    <row r="51" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Z50" s="63"/>
+      <c r="AA50" s="63"/>
+    </row>
+    <row r="51" spans="2:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="F51" s="63"/>
-      <c r="G51" s="9" t="s">
+      <c r="U51" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="H51" s="5"/>
-      <c r="I51" s="5"/>
-      <c r="J51" s="9" t="s">
+      <c r="V51" s="5"/>
+      <c r="W51" s="5"/>
+      <c r="X51" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="K51" s="9" t="s">
+      <c r="Y51" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="L51" s="63"/>
-      <c r="M51" s="63"/>
-      <c r="N51" s="63"/>
-    </row>
-    <row r="52" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Z51" s="63"/>
+      <c r="AA51" s="63"/>
+    </row>
+    <row r="52" spans="2:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="F52" s="63"/>
-      <c r="G52" s="9" t="s">
+      <c r="U52" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="H52" s="5"/>
-      <c r="I52" s="5"/>
-      <c r="J52" s="9" t="s">
+      <c r="V52" s="5"/>
+      <c r="W52" s="5"/>
+      <c r="X52" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="K52" s="9" t="s">
+      <c r="Y52" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="L52" s="63"/>
-      <c r="M52" s="63"/>
-      <c r="N52" s="63"/>
-    </row>
-    <row r="53" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Z52" s="63"/>
+      <c r="AA52" s="63"/>
+    </row>
+    <row r="53" spans="2:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="F53" s="63"/>
-      <c r="G53" s="9" t="s">
+      <c r="U53" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="H53" s="5"/>
-      <c r="I53" s="5"/>
-      <c r="J53" s="9" t="s">
+      <c r="V53" s="5"/>
+      <c r="W53" s="5"/>
+      <c r="X53" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="K53" s="9" t="s">
+      <c r="Y53" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="L53" s="63"/>
-      <c r="M53" s="63"/>
-      <c r="N53" s="63"/>
-    </row>
-    <row r="54" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Z53" s="63"/>
+      <c r="AA53" s="63"/>
+    </row>
+    <row r="54" spans="2:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="F54" s="63"/>
-      <c r="G54" s="9" t="s">
+      <c r="U54" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="H54" s="5"/>
-      <c r="I54" s="5"/>
-      <c r="J54" s="9" t="s">
+      <c r="V54" s="5"/>
+      <c r="W54" s="5"/>
+      <c r="X54" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="K54" s="9" t="s">
+      <c r="Y54" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="L54" s="63"/>
-      <c r="M54" s="63"/>
-      <c r="N54" s="63"/>
-    </row>
-    <row r="55" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Z54" s="63"/>
+      <c r="AA54" s="63"/>
+    </row>
+    <row r="55" spans="2:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="F55" s="63"/>
-      <c r="G55" s="9" t="s">
+      <c r="U55" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="H55" s="5"/>
-      <c r="I55" s="5"/>
-      <c r="J55" s="9" t="s">
+      <c r="V55" s="5"/>
+      <c r="W55" s="5"/>
+      <c r="X55" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="K55" s="9" t="s">
+      <c r="Y55" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="L55" s="63"/>
-      <c r="M55" s="63"/>
-      <c r="N55" s="63"/>
-    </row>
-    <row r="56" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Z55" s="63"/>
+      <c r="AA55" s="63"/>
+    </row>
+    <row r="56" spans="2:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="F56" s="63"/>
-      <c r="G56" s="9" t="s">
+      <c r="U56" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="H56" s="5"/>
-      <c r="I56" s="5"/>
-      <c r="J56" s="9" t="s">
+      <c r="V56" s="5"/>
+      <c r="W56" s="5"/>
+      <c r="X56" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="K56" s="9" t="s">
+      <c r="Y56" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="L56" s="63"/>
-      <c r="M56" s="63"/>
-      <c r="N56" s="63"/>
-    </row>
-    <row r="57" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Z56" s="63"/>
+      <c r="AA56" s="63"/>
+    </row>
+    <row r="57" spans="2:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="F57" s="63"/>
-      <c r="G57" s="9" t="s">
+      <c r="U57" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="H57" s="5"/>
-      <c r="I57" s="5"/>
-      <c r="J57" s="9" t="s">
+      <c r="V57" s="5"/>
+      <c r="W57" s="5"/>
+      <c r="X57" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="K57" s="9" t="s">
+      <c r="Y57" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="L57" s="63"/>
-      <c r="M57" s="63"/>
-      <c r="N57" s="63"/>
-    </row>
-    <row r="58" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Z57" s="63"/>
+      <c r="AA57" s="63"/>
+    </row>
+    <row r="58" spans="2:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="F58" s="63"/>
-      <c r="G58" s="9" t="s">
+      <c r="U58" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="H58" s="5"/>
-      <c r="I58" s="5"/>
-      <c r="J58" s="9" t="s">
+      <c r="V58" s="5"/>
+      <c r="W58" s="5"/>
+      <c r="X58" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="K58" s="9" t="s">
+      <c r="Y58" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="L58" s="63"/>
-      <c r="M58" s="63"/>
-      <c r="N58" s="63"/>
-    </row>
-    <row r="59" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Z58" s="63"/>
+      <c r="AA58" s="63"/>
+    </row>
+    <row r="59" spans="2:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="F59" s="63"/>
-      <c r="G59" s="9" t="s">
+      <c r="U59" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="H59" s="5"/>
-      <c r="I59" s="5"/>
-      <c r="J59" s="9" t="s">
+      <c r="V59" s="5"/>
+      <c r="W59" s="5"/>
+      <c r="X59" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="K59" s="9" t="s">
+      <c r="Y59" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="L59" s="63"/>
-      <c r="M59" s="63"/>
-      <c r="N59" s="63"/>
-    </row>
-    <row r="60" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Z59" s="63"/>
+      <c r="AA59" s="63"/>
+    </row>
+    <row r="60" spans="2:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="F60" s="63"/>
-      <c r="G60" s="9" t="s">
+      <c r="U60" s="9" t="s">
         <v>208</v>
       </c>
-      <c r="H60" s="5"/>
-      <c r="I60" s="5"/>
-      <c r="J60" s="9" t="s">
+      <c r="V60" s="5"/>
+      <c r="W60" s="5"/>
+      <c r="X60" s="9" t="s">
         <v>208</v>
       </c>
-      <c r="K60" s="9" t="s">
+      <c r="Y60" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="L60" s="63"/>
-      <c r="M60" s="63"/>
-      <c r="N60" s="63"/>
-    </row>
-    <row r="61" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Z60" s="63"/>
+      <c r="AA60" s="63"/>
+    </row>
+    <row r="61" spans="2:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="F61" s="63"/>
-      <c r="G61" s="9" t="s">
+      <c r="U61" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="H61" s="5"/>
-      <c r="I61" s="5"/>
-      <c r="J61" s="9" t="s">
+      <c r="V61" s="5"/>
+      <c r="W61" s="5"/>
+      <c r="X61" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="K61" s="9" t="s">
+      <c r="Y61" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="L61" s="63"/>
-      <c r="M61" s="63"/>
-      <c r="N61" s="63"/>
-    </row>
-    <row r="62" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Z61" s="63"/>
+      <c r="AA61" s="63"/>
+    </row>
+    <row r="62" spans="2:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="F62" s="63"/>
-      <c r="G62" s="9" t="s">
+      <c r="U62" s="9" t="s">
         <v>209</v>
       </c>
-      <c r="H62" s="5"/>
-      <c r="I62" s="5"/>
-      <c r="J62" s="9" t="s">
+      <c r="V62" s="5"/>
+      <c r="W62" s="5"/>
+      <c r="X62" s="9" t="s">
         <v>209</v>
       </c>
-      <c r="K62" s="9" t="s">
+      <c r="Y62" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="L62" s="63"/>
-      <c r="M62" s="63"/>
-      <c r="N62" s="63"/>
-    </row>
-    <row r="63" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Z62" s="63"/>
+      <c r="AA62" s="63"/>
+    </row>
+    <row r="63" spans="2:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="F63" s="63"/>
-      <c r="G63" s="9" t="s">
+      <c r="U63" s="9" t="s">
         <v>210</v>
       </c>
-      <c r="H63" s="5"/>
-      <c r="I63" s="5"/>
-      <c r="J63" s="9" t="s">
+      <c r="V63" s="5"/>
+      <c r="W63" s="5"/>
+      <c r="X63" s="9" t="s">
         <v>210</v>
       </c>
-      <c r="K63" s="9" t="s">
+      <c r="Y63" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="L63" s="63"/>
-      <c r="M63" s="63"/>
-      <c r="N63" s="63"/>
-    </row>
-    <row r="64" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Z63" s="63"/>
+      <c r="AA63" s="63"/>
+    </row>
+    <row r="64" spans="2:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="F64" s="63"/>
       <c r="H64" s="63"/>
       <c r="I64" s="63"/>
@@ -19898,16 +20072,19 @@
       <c r="G77" s="9"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C48:N48"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5B3E4D6-082C-4FC5-9A0B-7416C52470AD}">
-  <dimension ref="A2:N32"/>
+  <dimension ref="A2:N35"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20954,7 +21131,29 @@
       <c r="K32" s="8"/>
       <c r="L32" s="8"/>
     </row>
+    <row r="35" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>31</v>
+      </c>
+      <c r="C35" s="95" t="s">
+        <v>248</v>
+      </c>
+      <c r="D35" s="95"/>
+      <c r="E35" s="95"/>
+      <c r="F35" s="95"/>
+      <c r="G35" s="95"/>
+      <c r="H35" s="95"/>
+      <c r="I35" s="95"/>
+      <c r="J35" s="95"/>
+      <c r="K35" s="95"/>
+      <c r="L35" s="95"/>
+      <c r="M35" s="95"/>
+      <c r="N35" s="95"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C35:N35"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>